<commit_message>
Added negatives to diameter/radius/angles for right turns.
</commit_message>
<xml_diff>
--- a/motion_measurements.xlsx
+++ b/motion_measurements.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ajoy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JShannon\Documents\~Work\SDC\HarCar\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -529,10 +529,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$4</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>-1</c:v>
                 </c:pt>
@@ -542,15 +542,24 @@
                 <c:pt idx="2">
                   <c:v>-0.5</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$4</c:f>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>19.855214369321057</c:v>
                 </c:pt>
@@ -559,6 +568,15 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11.447167611611299</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.6567916505189224</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14.574216198038739</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-18.703101839365477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1866,16 +1884,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1896,16 +1914,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2193,7 +2211,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="X29" sqref="X29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2293,19 +2311,19 @@
         <v>0.5</v>
       </c>
       <c r="C5">
-        <v>3.82</v>
+        <v>-3.82</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>1.91</v>
+        <v>-1.91</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>0.16854280948065278</v>
+        <v>-0.16854280948065278</v>
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>9.6567916505189224</v>
+        <v>-9.6567916505189224</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2313,19 +2331,19 @@
         <v>0.75</v>
       </c>
       <c r="C6">
-        <v>2.5</v>
+        <v>-2.5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>1.25</v>
+        <v>-1.25</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>0.25436805855326594</v>
+        <v>-0.25436805855326594</v>
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>14.574216198038739</v>
+        <v>-14.574216198038739</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2333,19 +2351,19 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.92</v>
+        <v>-1.92</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.96</v>
+        <v>-0.96</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0.32643070743273517</v>
+        <v>-0.32643070743273517</v>
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>18.703101839365477</v>
+        <v>-18.703101839365477</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>